<commit_message>
Add dependencies, Admin-Role, not complete
</commit_message>
<xml_diff>
--- a/04-Project Source Code/Project Structure Design.xlsx
+++ b/04-Project Source Code/Project Structure Design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FinalProject\CampusMarket\04-Project Source Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3C99E1F-7357-4107-80EB-C79266A09B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA887510-A7C6-40E1-B571-D016A9B93078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>DuShopProject</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,14 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>com.dushop.admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.dushop.site</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DuShopWebParent</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -75,15 +67,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>src.main</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>resources</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>templates</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src.main.com.dushop.admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src.main.com.dushop.site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> - index.html  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The .html file for the home page of back end.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -91,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +121,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -163,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -198,6 +213,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -480,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -492,11 +510,13 @@
     <col min="2" max="3" width="4.625" style="10" customWidth="1"/>
     <col min="4" max="5" width="5.5" style="10" customWidth="1"/>
     <col min="6" max="6" width="5.75" style="10" customWidth="1"/>
-    <col min="7" max="10" width="9" style="10"/>
+    <col min="7" max="7" width="12.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="3.625" style="10" customWidth="1"/>
+    <col min="9" max="16" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -509,8 +529,14 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="12" t="s">
@@ -523,8 +549,14 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7"/>
@@ -532,81 +564,115 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5"/>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -614,147 +680,255 @@
       <c r="E10" s="7"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="E13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="7"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E21" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E22" s="9"/>
-      <c r="F22" s="4" t="s">
+      <c r="G21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E24" s="9"/>
+      <c r="F24" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G25" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>